<commit_message>
Completed Scraping,Filtering,Insertion process, completed updating process, made searchdate dynamic
</commit_message>
<xml_diff>
--- a/new_questions.xlsx
+++ b/new_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giou2\PycharmProjects\thesiswebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B59DF0-7A51-4C59-99E0-4D3A352721E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96783CAF-8D4E-41A3-88EA-4D1D03CD3D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4889,8 +4889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q204"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>